<commit_message>
end of day at ARC office
</commit_message>
<xml_diff>
--- a/data/iroc_response.xlsx
+++ b/data/iroc_response.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="18195" windowHeight="10995"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="18195" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="iroc_response" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="730">
   <si>
     <t>ARC_num</t>
   </si>
@@ -2202,6 +2202,9 @@
   </si>
   <si>
     <t>HKG</t>
+  </si>
+  <si>
+    <t>SXM</t>
   </si>
 </sst>
 </file>
@@ -3033,8 +3036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
-      <selection activeCell="E384" sqref="E384"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="F390" sqref="F390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14476,9 +14479,8 @@
       <c r="E372" t="s">
         <v>66</v>
       </c>
-      <c r="F372" t="e">
-        <f>VLOOKUP(E372,Sheet1!$A$2:$B$215,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="F372" t="s">
+        <v>729</v>
       </c>
       <c r="H372">
         <v>9000</v>

</xml_diff>